<commit_message>
idealo change html code
</commit_message>
<xml_diff>
--- a/Achat_lego.xlsx
+++ b/Achat_lego.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin\Documents\GitHub\bot-idealo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E494C87-0175-489A-A854-84DBB9E07F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8341BBE9-58F0-43A6-9E69-86F7B23A5591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -152,13 +152,70 @@
   </si>
   <si>
     <t>407-7291269-5461132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEGO Star Wars 75224 Sith Infiltrator™ Microfighter </t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/6434584/lego-star-wars-microvaisseau-sith-infiltrator-75224.html</t>
+  </si>
+  <si>
+    <t>Spiel &amp; Modellbau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEGO® 75345 Star Wars™ 501st Clone Troopers™ Battle Pack </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEGO Star Wars 75195 - Ski Speeder vs. First Order Walker Microfighters </t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/202257135/lego-star-wars-pack-de-combat-des-clone-troopers-de-la-501eme-legion-75345.html</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/5912809/lego-star-wars-microfighter-ski-speeder-vs-quadripode-du-premier-ordre-75195.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEGO® 75333 Star Wars™ Obi-Wan Kenobis Jedi Starfighter™ </t>
+  </si>
+  <si>
+    <t>5951-8985185-52</t>
+  </si>
+  <si>
+    <t>exemplaire</t>
+  </si>
+  <si>
+    <t>Le robot Boba Fett™ V29</t>
+  </si>
+  <si>
+    <t>Le robot Stormtrooper™ V29</t>
+  </si>
+  <si>
+    <t>Le robot Dark Vador V29</t>
+  </si>
+  <si>
+    <t>Pack de combat des Clone Tro.. V29</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/202887782/lego-star-wars-boba-fett-mech-75369.html</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/202887701/lego-star-wars-sturmtruppler-mech-75370.html</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/202887715/lego-star-wars-darth-vader-mech-75368.html</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/202873670/lego-star-wars-332-ahsoka-s-clone-trooper-battle-pack-75359.html</t>
+  </si>
+  <si>
+    <t>Prix unitaire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +228,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,7 +243,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -203,13 +266,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -514,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,11 +614,11 @@
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="5" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,25 +635,32 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -580,14 +676,20 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>75.989999999999995</v>
       </c>
-      <c r="K2" t="s">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2023</v>
       </c>
@@ -603,14 +705,20 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>39.799999999999997</v>
       </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
@@ -626,14 +734,20 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>50</v>
       </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -649,17 +763,20 @@
       <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>15.8</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="K5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -675,17 +792,20 @@
       <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>19.989999999999998</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -701,17 +821,20 @@
       <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2023</v>
       </c>
@@ -724,17 +847,20 @@
       <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>14</v>
       </c>
-      <c r="K8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2023</v>
       </c>
@@ -747,17 +873,20 @@
       <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2023</v>
       </c>
@@ -773,17 +902,20 @@
       <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>14</v>
       </c>
-      <c r="K10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2023</v>
       </c>
@@ -799,17 +931,20 @@
       <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>44.99</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>14</v>
       </c>
-      <c r="K11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -825,17 +960,20 @@
       <c r="E12" t="s">
         <v>35</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>17.489999999999998</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>14</v>
       </c>
-      <c r="K12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2023</v>
       </c>
@@ -851,17 +989,20 @@
       <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>34.99</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>14</v>
       </c>
-      <c r="K13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2023</v>
       </c>
@@ -877,17 +1018,20 @@
       <c r="E14" t="s">
         <v>35</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>44.994999999999997</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>14</v>
       </c>
-      <c r="K14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -903,17 +1047,20 @@
       <c r="E15" t="s">
         <v>35</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>89.99</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>14</v>
       </c>
-      <c r="K15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2023</v>
       </c>
@@ -932,57 +1079,238 @@
       <c r="F16">
         <v>59</v>
       </c>
-      <c r="K16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>177</v>
+      </c>
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2023</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>75089</v>
+        <v>75224</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17">
+        <v>46</v>
+      </c>
+      <c r="G17">
+        <v>13.9</v>
+      </c>
+      <c r="L17" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2023</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18">
+        <v>75345</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18">
+        <v>15.99</v>
+      </c>
+      <c r="L18" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2023</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19">
+        <v>75195</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19">
+        <v>28</v>
+      </c>
+      <c r="L19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2023</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <v>75333</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20">
+        <v>27.99</v>
+      </c>
+      <c r="L20" t="s">
+        <v>52</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2023</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21">
+        <v>75369</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21">
+        <v>15.99</v>
+      </c>
+      <c r="G21">
+        <v>79.95</v>
+      </c>
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2023</v>
+      </c>
+      <c r="B22" t="s">
         <v>59</v>
       </c>
-      <c r="K17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2023</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>75089</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18">
-        <v>59</v>
-      </c>
-      <c r="K18" t="s">
-        <v>23</v>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22">
+        <v>75370</v>
+      </c>
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>15.99</v>
+      </c>
+      <c r="G22">
+        <v>79.95</v>
+      </c>
+      <c r="L22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2023</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23">
+        <v>75368</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>15.99</v>
+      </c>
+      <c r="G23">
+        <v>79.95</v>
+      </c>
+      <c r="L23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2023</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24">
+        <v>75359</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24">
+        <v>0.99</v>
+      </c>
+      <c r="G24">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L24" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2.  Il est possible que le lego soit assez rare pour qu'il n'apparaisse pas dans idéalo, donc on doit prendre le prix ailleur `à def`.     3.  Il est possible que le logi soit assez rare pour qu'il n'apparaisse quand état d'occasion, donc on doit prendre le prix ailleur `à def`.
</commit_message>
<xml_diff>
--- a/Achat_lego.xlsx
+++ b/Achat_lego.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin\Documents\GitHub\bot-idealo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A9C56C-8EB2-413B-A1B6-56E120E4C869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8DC909-44AF-43A0-894E-41E3A2FB448F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="630" windowWidth="19200" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,7 +2068,7 @@
       <c r="G48">
         <v>80</v>
       </c>
-      <c r="H48" s="8"/>
+      <c r="H48" s="7"/>
       <c r="L48" t="s">
         <v>21</v>
       </c>
@@ -2095,7 +2095,7 @@
       <c r="G49">
         <v>80</v>
       </c>
-      <c r="H49" s="8"/>
+      <c r="H49" s="7"/>
       <c r="L49" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
4.  Garder les couleurs de l'input file sur la colonne `Stoké` ✅
</commit_message>
<xml_diff>
--- a/Achat_lego.xlsx
+++ b/Achat_lego.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin\Documents\GitHub\bot-idealo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8DC909-44AF-43A0-894E-41E3A2FB448F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D2FF5D-1572-486D-BAA2-C83B9E385A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="630" windowWidth="19200" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -333,13 +333,19 @@
   </si>
   <si>
     <t>anacour</t>
+  </si>
+  <si>
+    <t>Etat de la commande</t>
+  </si>
+  <si>
+    <t>Couleur etat de la commande</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,12 +357,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -400,7 +400,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -423,44 +423,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -770,22 +744,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="4" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,14 +801,20 @@
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -848,19 +833,19 @@
       <c r="G2">
         <v>75.989999999999995</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="4"/>
       <c r="L2" t="s">
         <v>41</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" t="s">
+      <c r="O2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2023</v>
       </c>
@@ -879,19 +864,19 @@
       <c r="G3">
         <v>39.799999999999997</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="4"/>
       <c r="L3" t="s">
         <v>21</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" t="s">
+      <c r="O3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
@@ -910,19 +895,19 @@
       <c r="G4">
         <v>50</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="4"/>
       <c r="L4" t="s">
         <v>21</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
-      <c r="P4" s="8"/>
-      <c r="Q4" t="s">
+      <c r="O4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -941,7 +926,7 @@
       <c r="G5">
         <v>15.8</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="4"/>
       <c r="L5" t="s">
         <v>21</v>
       </c>
@@ -949,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -968,7 +953,7 @@
       <c r="G6">
         <v>19.989999999999998</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="4"/>
       <c r="L6" t="s">
         <v>21</v>
       </c>
@@ -976,7 +961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -995,7 +980,7 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="4"/>
       <c r="L7" t="s">
         <v>21</v>
       </c>
@@ -1003,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2023</v>
       </c>
@@ -1019,7 +1004,7 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="4"/>
       <c r="L8" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2023</v>
       </c>
@@ -1043,7 +1028,7 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="4"/>
       <c r="L9" t="s">
         <v>21</v>
       </c>
@@ -1051,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2023</v>
       </c>
@@ -1070,7 +1055,7 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="4"/>
       <c r="L10" t="s">
         <v>21</v>
       </c>
@@ -1078,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2023</v>
       </c>
@@ -1097,7 +1082,7 @@
       <c r="G11">
         <v>44.99</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="4"/>
       <c r="L11" t="s">
         <v>21</v>
       </c>
@@ -1105,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -1124,7 +1109,7 @@
       <c r="G12">
         <v>17.489999999999998</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="4"/>
       <c r="L12" t="s">
         <v>21</v>
       </c>
@@ -1132,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2023</v>
       </c>
@@ -1151,7 +1136,7 @@
       <c r="G13">
         <v>34.99</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="4"/>
       <c r="L13" t="s">
         <v>21</v>
       </c>
@@ -1159,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2023</v>
       </c>
@@ -1178,7 +1163,7 @@
       <c r="G14">
         <v>44.994999999999997</v>
       </c>
-      <c r="H14" s="6"/>
+      <c r="H14" s="4"/>
       <c r="L14" t="s">
         <v>21</v>
       </c>
@@ -1186,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -1205,7 +1190,7 @@
       <c r="G15">
         <v>89.99</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="4"/>
       <c r="L15" t="s">
         <v>21</v>
       </c>
@@ -1213,7 +1198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2023</v>
       </c>
@@ -1235,7 +1220,7 @@
       <c r="G16">
         <v>177</v>
       </c>
-      <c r="H16" s="6"/>
+      <c r="H16" s="4"/>
       <c r="L16" t="s">
         <v>21</v>
       </c>
@@ -1262,7 +1247,7 @@
       <c r="G17">
         <v>13.9</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="4"/>
       <c r="L17" t="s">
         <v>50</v>
       </c>
@@ -1289,7 +1274,7 @@
       <c r="G18">
         <v>15.99</v>
       </c>
-      <c r="H18" s="6"/>
+      <c r="H18" s="4"/>
       <c r="L18" t="s">
         <v>50</v>
       </c>
@@ -1316,7 +1301,7 @@
       <c r="G19">
         <v>28</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="4"/>
       <c r="L19" t="s">
         <v>50</v>
       </c>
@@ -1343,7 +1328,7 @@
       <c r="G20">
         <v>27.99</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="4"/>
       <c r="L20" t="s">
         <v>50</v>
       </c>
@@ -1373,7 +1358,7 @@
       <c r="G21">
         <v>79.95</v>
       </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="4"/>
       <c r="L21" t="s">
         <v>21</v>
       </c>
@@ -1403,7 +1388,7 @@
       <c r="G22">
         <v>79.95</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="4"/>
       <c r="L22" t="s">
         <v>21</v>
       </c>
@@ -1433,7 +1418,7 @@
       <c r="G23">
         <v>79.95</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="4"/>
       <c r="L23" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1448,7 @@
       <c r="G24">
         <v>4.9000000000000004</v>
       </c>
-      <c r="H24" s="6"/>
+      <c r="H24" s="4"/>
       <c r="L24" t="s">
         <v>21</v>
       </c>
@@ -1475,10 +1460,10 @@
       <c r="A25">
         <v>2023</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="2">
         <v>75126</v>
       </c>
       <c r="E25" t="s">
@@ -1487,7 +1472,7 @@
       <c r="G25">
         <v>10</v>
       </c>
-      <c r="H25" s="8"/>
+      <c r="H25" s="6"/>
       <c r="L25" t="s">
         <v>21</v>
       </c>
@@ -1514,8 +1499,8 @@
       <c r="G26">
         <v>40</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="I26" s="9">
+      <c r="H26" s="5"/>
+      <c r="I26" s="7">
         <v>180</v>
       </c>
       <c r="L26" t="s">
@@ -1529,7 +1514,7 @@
       <c r="A27">
         <v>2023</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D27">
@@ -1541,7 +1526,7 @@
       <c r="G27">
         <v>57</v>
       </c>
-      <c r="H27" s="7"/>
+      <c r="H27" s="5"/>
       <c r="L27" t="s">
         <v>21</v>
       </c>
@@ -1553,7 +1538,7 @@
       <c r="A28">
         <v>2023</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D28">
@@ -1565,7 +1550,7 @@
       <c r="G28">
         <v>20</v>
       </c>
-      <c r="H28" s="7"/>
+      <c r="H28" s="5"/>
       <c r="L28" t="s">
         <v>21</v>
       </c>
@@ -1580,7 +1565,7 @@
       <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="2">
         <v>75235</v>
       </c>
       <c r="E29" t="s">
@@ -1589,7 +1574,7 @@
       <c r="G29">
         <v>30</v>
       </c>
-      <c r="H29" s="7"/>
+      <c r="H29" s="5"/>
       <c r="L29" t="s">
         <v>21</v>
       </c>
@@ -1604,7 +1589,7 @@
       <c r="B30" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="2">
         <v>75281</v>
       </c>
       <c r="E30" t="s">
@@ -1613,7 +1598,7 @@
       <c r="G30">
         <v>43</v>
       </c>
-      <c r="H30" s="7"/>
+      <c r="H30" s="5"/>
       <c r="L30" t="s">
         <v>21</v>
       </c>
@@ -1628,7 +1613,7 @@
       <c r="B31" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="2">
         <v>75246</v>
       </c>
       <c r="E31" t="s">
@@ -1637,7 +1622,7 @@
       <c r="G31">
         <v>24</v>
       </c>
-      <c r="H31" s="7"/>
+      <c r="H31" s="5"/>
       <c r="L31" t="s">
         <v>21</v>
       </c>
@@ -1652,7 +1637,7 @@
       <c r="B32" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="2">
         <v>75236</v>
       </c>
       <c r="E32" t="s">
@@ -1661,7 +1646,7 @@
       <c r="G32">
         <v>24</v>
       </c>
-      <c r="H32" s="7"/>
+      <c r="H32" s="5"/>
       <c r="L32" t="s">
         <v>21</v>
       </c>
@@ -1676,7 +1661,7 @@
       <c r="B33" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <v>75229</v>
       </c>
       <c r="E33" t="s">
@@ -1685,7 +1670,7 @@
       <c r="G33">
         <v>33</v>
       </c>
-      <c r="H33" s="7"/>
+      <c r="H33" s="5"/>
       <c r="L33" t="s">
         <v>21</v>
       </c>
@@ -1700,7 +1685,7 @@
       <c r="B34" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="2">
         <v>75177</v>
       </c>
       <c r="E34" t="s">
@@ -1709,7 +1694,7 @@
       <c r="G34">
         <v>48</v>
       </c>
-      <c r="H34" s="7"/>
+      <c r="H34" s="5"/>
       <c r="L34" t="s">
         <v>21</v>
       </c>
@@ -1724,7 +1709,7 @@
       <c r="B35" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="2">
         <v>75078</v>
       </c>
       <c r="E35" t="s">
@@ -1733,7 +1718,7 @@
       <c r="G35">
         <v>38</v>
       </c>
-      <c r="H35" s="7"/>
+      <c r="H35" s="5"/>
       <c r="L35" t="s">
         <v>21</v>
       </c>
@@ -1748,7 +1733,7 @@
       <c r="B36" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="2">
         <v>75039</v>
       </c>
       <c r="E36" t="s">
@@ -1757,7 +1742,7 @@
       <c r="G36">
         <v>69</v>
       </c>
-      <c r="H36" s="6"/>
+      <c r="H36" s="4"/>
       <c r="L36" t="s">
         <v>21</v>
       </c>
@@ -1772,7 +1757,7 @@
       <c r="B37" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="2">
         <v>75198</v>
       </c>
       <c r="E37" t="s">
@@ -1781,7 +1766,7 @@
       <c r="G37">
         <v>29</v>
       </c>
-      <c r="H37" s="7"/>
+      <c r="H37" s="5"/>
       <c r="L37" t="s">
         <v>21</v>
       </c>
@@ -1796,7 +1781,7 @@
       <c r="B38" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="2">
         <v>75215</v>
       </c>
       <c r="E38" t="s">
@@ -1805,7 +1790,7 @@
       <c r="G38">
         <v>60</v>
       </c>
-      <c r="H38" s="7"/>
+      <c r="H38" s="5"/>
       <c r="L38" t="s">
         <v>21</v>
       </c>
@@ -1820,7 +1805,7 @@
       <c r="B39" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="2">
         <v>75266</v>
       </c>
       <c r="E39" t="s">
@@ -1833,7 +1818,7 @@
         <f>F39*5</f>
         <v>99</v>
       </c>
-      <c r="H39" s="7"/>
+      <c r="H39" s="5"/>
       <c r="L39" t="s">
         <v>21</v>
       </c>
@@ -1845,10 +1830,10 @@
       <c r="A40">
         <v>2023</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="2">
         <v>75258</v>
       </c>
       <c r="E40" t="s">
@@ -1857,7 +1842,7 @@
       <c r="G40">
         <v>40</v>
       </c>
-      <c r="H40" s="7"/>
+      <c r="H40" s="5"/>
       <c r="L40" t="s">
         <v>21</v>
       </c>
@@ -1872,7 +1857,7 @@
       <c r="B41" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="2">
         <v>75299</v>
       </c>
       <c r="E41" t="s">
@@ -1881,7 +1866,7 @@
       <c r="G41">
         <v>28</v>
       </c>
-      <c r="H41" s="7"/>
+      <c r="H41" s="5"/>
       <c r="L41" t="s">
         <v>21</v>
       </c>
@@ -1896,7 +1881,7 @@
       <c r="B42" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="2">
         <v>75363</v>
       </c>
       <c r="E42" t="s">
@@ -1909,7 +1894,7 @@
         <f>F42*4</f>
         <v>47.6</v>
       </c>
-      <c r="H42" s="6"/>
+      <c r="H42" s="4"/>
       <c r="L42" t="s">
         <v>21</v>
       </c>
@@ -1933,7 +1918,7 @@
       <c r="G43">
         <v>23</v>
       </c>
-      <c r="H43" s="8"/>
+      <c r="H43" s="6"/>
       <c r="L43" t="s">
         <v>21</v>
       </c>
@@ -1948,7 +1933,7 @@
       <c r="A44">
         <v>2023</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D44">
@@ -1960,7 +1945,7 @@
       <c r="G44">
         <v>22</v>
       </c>
-      <c r="H44" s="8"/>
+      <c r="H44" s="6"/>
       <c r="L44" t="s">
         <v>21</v>
       </c>
@@ -1975,7 +1960,7 @@
       <c r="A45">
         <v>2023</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D45">
@@ -1987,7 +1972,7 @@
       <c r="G45">
         <v>23</v>
       </c>
-      <c r="H45" s="8"/>
+      <c r="H45" s="6"/>
       <c r="L45" t="s">
         <v>21</v>
       </c>
@@ -2002,7 +1987,7 @@
       <c r="A46">
         <v>2023</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D46">
@@ -2014,7 +1999,7 @@
       <c r="G46">
         <v>22</v>
       </c>
-      <c r="H46" s="8"/>
+      <c r="H46" s="6"/>
       <c r="L46" t="s">
         <v>21</v>
       </c>
@@ -2029,7 +2014,7 @@
       <c r="A47">
         <v>2023</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D47">
@@ -2041,7 +2026,7 @@
       <c r="G47">
         <v>22.5</v>
       </c>
-      <c r="H47" s="7"/>
+      <c r="H47" s="5"/>
       <c r="L47" t="s">
         <v>21</v>
       </c>
@@ -2068,7 +2053,7 @@
       <c r="G48">
         <v>80</v>
       </c>
-      <c r="H48" s="7"/>
+      <c r="H48" s="5"/>
       <c r="L48" t="s">
         <v>21</v>
       </c>
@@ -2095,7 +2080,7 @@
       <c r="G49">
         <v>80</v>
       </c>
-      <c r="H49" s="7"/>
+      <c r="H49" s="5"/>
       <c r="L49" t="s">
         <v>21</v>
       </c>
@@ -2122,7 +2107,7 @@
       <c r="G50">
         <v>30</v>
       </c>
-      <c r="H50" s="8"/>
+      <c r="H50" s="6"/>
       <c r="L50" t="s">
         <v>21</v>
       </c>
@@ -2149,7 +2134,7 @@
       <c r="G51">
         <v>25</v>
       </c>
-      <c r="H51" s="8"/>
+      <c r="H51" s="6"/>
       <c r="L51" t="s">
         <v>21</v>
       </c>
@@ -2176,7 +2161,7 @@
       <c r="G52">
         <v>19</v>
       </c>
-      <c r="H52" s="7"/>
+      <c r="H52" s="5"/>
       <c r="L52" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Ajout dune nouvelle col
</commit_message>
<xml_diff>
--- a/Achat_lego.xlsx
+++ b/Achat_lego.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin\Documents\GitHub\bot-idealo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D2FF5D-1572-486D-BAA2-C83B9E385A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17D0769-27E9-49D5-B31E-FE1F21E12CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -339,6 +339,24 @@
   </si>
   <si>
     <t>Couleur etat de la commande</t>
+  </si>
+  <si>
+    <t>adlge</t>
+  </si>
+  <si>
+    <t>v.loretguilbaud</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/4970507/lego-star-wars-eclipse-fighter-75145.html</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/201088979/lego-star-wars-microfighter-faucon-millenium-75295.html</t>
+  </si>
+  <si>
+    <t>Livraison</t>
+  </si>
+  <si>
+    <t>King jouet</t>
   </si>
 </sst>
 </file>
@@ -744,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,11 +778,13 @@
     <col min="9" max="9" width="17.42578125" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
-    <col min="16" max="16" width="28.5703125" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" customWidth="1"/>
+    <col min="17" max="17" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,13 +828,16 @@
         <v>61</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -840,12 +863,12 @@
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>84</v>
       </c>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2023</v>
       </c>
@@ -871,12 +894,12 @@
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
@@ -902,12 +925,12 @@
       <c r="M4">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>86</v>
       </c>
-      <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -934,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -961,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -988,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2023</v>
       </c>
@@ -1012,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2023</v>
       </c>
@@ -1036,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2023</v>
       </c>
@@ -1063,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2023</v>
       </c>
@@ -1090,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -1117,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2023</v>
       </c>
@@ -1144,7 +1167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2023</v>
       </c>
@@ -1171,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2023</v>
       </c>
@@ -1198,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2023</v>
       </c>
@@ -1228,7 +1251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -1255,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2023</v>
       </c>
@@ -1282,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2023</v>
       </c>
@@ -1309,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2023</v>
       </c>
@@ -1336,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2023</v>
       </c>
@@ -1366,7 +1389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2023</v>
       </c>
@@ -1396,7 +1419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2023</v>
       </c>
@@ -1426,7 +1449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2023</v>
       </c>
@@ -1456,7 +1479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2023</v>
       </c>
@@ -1482,8 +1505,11 @@
       <c r="N25" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2023</v>
       </c>
@@ -1509,8 +1535,11 @@
       <c r="M26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2023</v>
       </c>
@@ -1533,8 +1562,11 @@
       <c r="M27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2023</v>
       </c>
@@ -1557,8 +1589,11 @@
       <c r="M28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2023</v>
       </c>
@@ -1581,8 +1616,11 @@
       <c r="M29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2023</v>
       </c>
@@ -1605,8 +1643,11 @@
       <c r="M30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2023</v>
       </c>
@@ -1629,8 +1670,11 @@
       <c r="M31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2023</v>
       </c>
@@ -1653,8 +1697,11 @@
       <c r="M32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2023</v>
       </c>
@@ -1677,8 +1724,11 @@
       <c r="M33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2023</v>
       </c>
@@ -1701,8 +1751,11 @@
       <c r="M34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2023</v>
       </c>
@@ -1725,8 +1778,11 @@
       <c r="M35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2023</v>
       </c>
@@ -1749,8 +1805,11 @@
       <c r="M36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2023</v>
       </c>
@@ -1773,8 +1832,11 @@
       <c r="M37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2023</v>
       </c>
@@ -1797,8 +1859,11 @@
       <c r="M38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2023</v>
       </c>
@@ -1825,8 +1890,11 @@
       <c r="M39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2023</v>
       </c>
@@ -1849,8 +1917,11 @@
       <c r="M40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2023</v>
       </c>
@@ -1873,8 +1944,11 @@
       <c r="M41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2023</v>
       </c>
@@ -1901,8 +1975,11 @@
       <c r="M42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2023</v>
       </c>
@@ -1928,8 +2005,11 @@
       <c r="N43" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2023</v>
       </c>
@@ -1955,8 +2035,11 @@
       <c r="N44" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2023</v>
       </c>
@@ -1982,8 +2065,11 @@
       <c r="N45" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2023</v>
       </c>
@@ -2009,8 +2095,11 @@
       <c r="N46" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2023</v>
       </c>
@@ -2036,8 +2125,11 @@
       <c r="N47" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2023</v>
       </c>
@@ -2063,8 +2155,11 @@
       <c r="N48" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2023</v>
       </c>
@@ -2090,8 +2185,11 @@
       <c r="N49" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2023</v>
       </c>
@@ -2117,8 +2215,11 @@
       <c r="N50" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2023</v>
       </c>
@@ -2144,8 +2245,11 @@
       <c r="N51" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2023</v>
       </c>
@@ -2170,6 +2274,69 @@
       </c>
       <c r="N52" t="s">
         <v>98</v>
+      </c>
+      <c r="O52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2023</v>
+      </c>
+      <c r="B53" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53">
+        <v>75145</v>
+      </c>
+      <c r="E53" t="s">
+        <v>63</v>
+      </c>
+      <c r="G53">
+        <v>35.15</v>
+      </c>
+      <c r="H53" s="6"/>
+      <c r="L53" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53" t="s">
+        <v>102</v>
+      </c>
+      <c r="O53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2023</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54">
+        <v>75295</v>
+      </c>
+      <c r="E54" t="s">
+        <v>63</v>
+      </c>
+      <c r="G54">
+        <v>8.83</v>
+      </c>
+      <c r="H54" s="6"/>
+      <c r="L54" t="s">
+        <v>21</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54" t="s">
+        <v>103</v>
+      </c>
+      <c r="O54" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nouvelle etat de commande : point relais
</commit_message>
<xml_diff>
--- a/Achat_lego.xlsx
+++ b/Achat_lego.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin\Documents\GitHub\bot-idealo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17D0769-27E9-49D5-B31E-FE1F21E12CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C169B661-369A-407F-A153-4DF193EBAECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="115">
   <si>
     <t>Date</t>
   </si>
@@ -357,6 +357,27 @@
   </si>
   <si>
     <t>King jouet</t>
+  </si>
+  <si>
+    <t>nestarit</t>
+  </si>
+  <si>
+    <t>LEGO Microfighter Navette de Kylo Ren™</t>
+  </si>
+  <si>
+    <t>Chez moi</t>
+  </si>
+  <si>
+    <t>B07W8XYZ2X</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/6982410/lego-star-wars-microfighter-navette-de-kylo-ren-75264.html</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/6982375/lego-star-wars-microfighter-y-wing-de-la-resistance-75263.html</t>
+  </si>
+  <si>
+    <t>point relais</t>
   </si>
 </sst>
 </file>
@@ -392,7 +413,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,6 +435,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -459,6 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -762,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q54"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,9 +923,9 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q3" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -926,9 +954,9 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q4" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -956,6 +984,10 @@
       <c r="M5">
         <v>1</v>
       </c>
+      <c r="P5" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1525,7 +1557,7 @@
       <c r="G26">
         <v>40</v>
       </c>
-      <c r="H26" s="5"/>
+      <c r="H26" s="4"/>
       <c r="I26" s="7">
         <v>180</v>
       </c>
@@ -1555,7 +1587,7 @@
       <c r="G27">
         <v>57</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="4"/>
       <c r="L27" t="s">
         <v>21</v>
       </c>
@@ -1582,7 +1614,7 @@
       <c r="G28">
         <v>20</v>
       </c>
-      <c r="H28" s="5"/>
+      <c r="H28" s="4"/>
       <c r="L28" t="s">
         <v>21</v>
       </c>
@@ -1609,7 +1641,7 @@
       <c r="G29">
         <v>30</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="4"/>
       <c r="L29" t="s">
         <v>21</v>
       </c>
@@ -1636,7 +1668,7 @@
       <c r="G30">
         <v>43</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="4"/>
       <c r="L30" t="s">
         <v>21</v>
       </c>
@@ -1663,7 +1695,7 @@
       <c r="G31">
         <v>24</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="4"/>
       <c r="L31" t="s">
         <v>21</v>
       </c>
@@ -1690,7 +1722,7 @@
       <c r="G32">
         <v>24</v>
       </c>
-      <c r="H32" s="5"/>
+      <c r="H32" s="4"/>
       <c r="L32" t="s">
         <v>21</v>
       </c>
@@ -1717,7 +1749,7 @@
       <c r="G33">
         <v>33</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="4"/>
       <c r="L33" t="s">
         <v>21</v>
       </c>
@@ -1825,7 +1857,7 @@
       <c r="G37">
         <v>29</v>
       </c>
-      <c r="H37" s="5"/>
+      <c r="H37" s="4"/>
       <c r="L37" t="s">
         <v>21</v>
       </c>
@@ -1852,7 +1884,7 @@
       <c r="G38">
         <v>60</v>
       </c>
-      <c r="H38" s="5"/>
+      <c r="H38" s="4"/>
       <c r="L38" t="s">
         <v>21</v>
       </c>
@@ -1883,7 +1915,7 @@
         <f>F39*5</f>
         <v>99</v>
       </c>
-      <c r="H39" s="5"/>
+      <c r="H39" s="4"/>
       <c r="L39" t="s">
         <v>21</v>
       </c>
@@ -1937,7 +1969,7 @@
       <c r="G41">
         <v>28</v>
       </c>
-      <c r="H41" s="5"/>
+      <c r="H41" s="8"/>
       <c r="L41" t="s">
         <v>21</v>
       </c>
@@ -2205,7 +2237,7 @@
       <c r="G50">
         <v>30</v>
       </c>
-      <c r="H50" s="6"/>
+      <c r="H50" s="5"/>
       <c r="L50" t="s">
         <v>21</v>
       </c>
@@ -2235,7 +2267,7 @@
       <c r="G51">
         <v>25</v>
       </c>
-      <c r="H51" s="6"/>
+      <c r="H51" s="5"/>
       <c r="L51" t="s">
         <v>21</v>
       </c>
@@ -2337,6 +2369,102 @@
       </c>
       <c r="O54" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2023</v>
+      </c>
+      <c r="B55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55">
+        <v>75246</v>
+      </c>
+      <c r="E55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G55">
+        <v>25</v>
+      </c>
+      <c r="H55" s="6"/>
+      <c r="L55" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55" t="s">
+        <v>108</v>
+      </c>
+      <c r="O55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2023</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56">
+        <v>75263</v>
+      </c>
+      <c r="E56" t="s">
+        <v>63</v>
+      </c>
+      <c r="G56">
+        <v>11.13</v>
+      </c>
+      <c r="H56" s="6"/>
+      <c r="L56" t="s">
+        <v>21</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56" t="s">
+        <v>108</v>
+      </c>
+      <c r="O56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2023</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57">
+        <v>75264</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57">
+        <v>29.83</v>
+      </c>
+      <c r="G57">
+        <v>119.32</v>
+      </c>
+      <c r="H57" s="6"/>
+      <c r="L57" t="s">
+        <v>21</v>
+      </c>
+      <c r="M57">
+        <v>4</v>
+      </c>
+      <c r="N57" t="s">
+        <v>111</v>
+      </c>
+      <c r="O57" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bar de progression, nouveau lego
</commit_message>
<xml_diff>
--- a/Achat_lego.xlsx
+++ b/Achat_lego.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin\Documents\GitHub\bot-idealo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEA9EE8-49D7-4189-9473-859113823D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9E2FDE-23C0-4EB0-82AE-D91E26F93BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="121">
   <si>
     <t>Date</t>
   </si>
@@ -378,6 +378,24 @@
   </si>
   <si>
     <t>point relais</t>
+  </si>
+  <si>
+    <t>lidiacely</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/201745502/lego-star-wars-pack-de-combat-snowtrooper-75320.html</t>
+  </si>
+  <si>
+    <t>geekoliv</t>
+  </si>
+  <si>
+    <t>janguifett</t>
+  </si>
+  <si>
+    <t>krispjek</t>
+  </si>
+  <si>
+    <t>https://www.idealo.fr/prix/4922107/lego-star-wars-at-dp-75130.html</t>
   </si>
 </sst>
 </file>
@@ -790,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55:H56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K11" sqref="C10:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,6 +1801,9 @@
       <c r="M34">
         <v>1</v>
       </c>
+      <c r="N34" t="s">
+        <v>117</v>
+      </c>
       <c r="O34" t="s">
         <v>107</v>
       </c>
@@ -1809,6 +1830,9 @@
       </c>
       <c r="M35">
         <v>1</v>
+      </c>
+      <c r="N35" t="s">
+        <v>117</v>
       </c>
       <c r="O35" t="s">
         <v>107</v>
@@ -1942,7 +1966,7 @@
       <c r="G40">
         <v>40</v>
       </c>
-      <c r="H40" s="5"/>
+      <c r="H40" s="4"/>
       <c r="L40" t="s">
         <v>21</v>
       </c>
@@ -1969,7 +1993,7 @@
       <c r="G41">
         <v>28</v>
       </c>
-      <c r="H41" s="8"/>
+      <c r="H41" s="4"/>
       <c r="L41" t="s">
         <v>21</v>
       </c>
@@ -2027,7 +2051,7 @@
       <c r="G43">
         <v>23</v>
       </c>
-      <c r="H43" s="6"/>
+      <c r="H43" s="5"/>
       <c r="L43" t="s">
         <v>21</v>
       </c>
@@ -2147,7 +2171,7 @@
       <c r="G47">
         <v>22.5</v>
       </c>
-      <c r="H47" s="5"/>
+      <c r="H47" s="4"/>
       <c r="L47" t="s">
         <v>21</v>
       </c>
@@ -2177,7 +2201,7 @@
       <c r="G48">
         <v>80</v>
       </c>
-      <c r="H48" s="5"/>
+      <c r="H48" s="4"/>
       <c r="L48" t="s">
         <v>21</v>
       </c>
@@ -2207,7 +2231,7 @@
       <c r="G49">
         <v>80</v>
       </c>
-      <c r="H49" s="5"/>
+      <c r="H49" s="4"/>
       <c r="L49" t="s">
         <v>21</v>
       </c>
@@ -2297,7 +2321,7 @@
       <c r="G52">
         <v>19</v>
       </c>
-      <c r="H52" s="5"/>
+      <c r="H52" s="4"/>
       <c r="L52" t="s">
         <v>21</v>
       </c>
@@ -2327,7 +2351,7 @@
       <c r="G53">
         <v>35.15</v>
       </c>
-      <c r="H53" s="6"/>
+      <c r="H53" s="5"/>
       <c r="L53" t="s">
         <v>21</v>
       </c>
@@ -2465,6 +2489,156 @@
       </c>
       <c r="O57" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2023</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58">
+        <v>75363</v>
+      </c>
+      <c r="E58" t="s">
+        <v>63</v>
+      </c>
+      <c r="G58">
+        <v>8.08</v>
+      </c>
+      <c r="H58" s="6"/>
+      <c r="L58" t="s">
+        <v>21</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58" t="s">
+        <v>115</v>
+      </c>
+      <c r="O58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2023</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59">
+        <v>75345</v>
+      </c>
+      <c r="E59" t="s">
+        <v>63</v>
+      </c>
+      <c r="G59">
+        <v>15</v>
+      </c>
+      <c r="H59" s="6"/>
+      <c r="L59" t="s">
+        <v>21</v>
+      </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59" t="s">
+        <v>115</v>
+      </c>
+      <c r="O59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2023</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60">
+        <v>75320</v>
+      </c>
+      <c r="E60" t="s">
+        <v>63</v>
+      </c>
+      <c r="G60">
+        <v>12</v>
+      </c>
+      <c r="H60" s="6"/>
+      <c r="L60" t="s">
+        <v>21</v>
+      </c>
+      <c r="M60">
+        <v>1</v>
+      </c>
+      <c r="N60" t="s">
+        <v>115</v>
+      </c>
+      <c r="O60" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2023</v>
+      </c>
+      <c r="B61" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61">
+        <v>40451</v>
+      </c>
+      <c r="E61" t="s">
+        <v>63</v>
+      </c>
+      <c r="G61">
+        <v>22.88</v>
+      </c>
+      <c r="H61" s="6"/>
+      <c r="L61" t="s">
+        <v>21</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+      <c r="N61" t="s">
+        <v>118</v>
+      </c>
+      <c r="O61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2023</v>
+      </c>
+      <c r="B62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62">
+        <v>75130</v>
+      </c>
+      <c r="E62" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62">
+        <v>19.34</v>
+      </c>
+      <c r="H62" s="6"/>
+      <c r="L62" t="s">
+        <v>21</v>
+      </c>
+      <c r="M62">
+        <v>1</v>
+      </c>
+      <c r="N62" t="s">
+        <v>119</v>
+      </c>
+      <c r="O62" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2476,8 +2650,9 @@
     <hyperlink ref="B46" r:id="rId5" xr:uid="{10D73F36-906E-4AE2-A627-A3BE4887FAC3}"/>
     <hyperlink ref="B45" r:id="rId6" display="https://www.idealo.fr/prix/201976964/lego-star-wars-le-chasseur-jedi-d-obi-wan-kenobi-75333.html" xr:uid="{9A11A668-BD64-4A8E-A054-42B28CD6C222}"/>
     <hyperlink ref="B44" r:id="rId7" display="https://www.idealo.fr/prix/202464341/lego-star-wars-pirate-snub-fighter-75346.html" xr:uid="{2E4AC1F4-0EE7-4272-B01D-51818A62A89B}"/>
+    <hyperlink ref="B59" r:id="rId8" xr:uid="{C9598487-F01B-4373-B6D4-5325B7433A8B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>